<commit_message>
run and notate marrbyregion regs
</commit_message>
<xml_diff>
--- a/notes/explore-results.xlsx
+++ b/notes/explore-results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="77">
   <si>
     <t>Universe</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Male migs to N</t>
   </si>
   <si>
-    <t>erscore50</t>
-  </si>
-  <si>
-    <t>DD: MWithinNorth MToNorth</t>
-  </si>
-  <si>
     <t>Female migs to N</t>
   </si>
   <si>
@@ -160,6 +154,102 @@
   </si>
   <si>
     <t>PLANNED SPECIFICATION on basis of explorations above</t>
+  </si>
+  <si>
+    <t>TO-DO: Consider splitting 'North' into multiple regions</t>
+  </si>
+  <si>
+    <t>occscore_real</t>
+  </si>
+  <si>
+    <t>DD: MWithinNorth</t>
+  </si>
+  <si>
+    <t>tWMAA ~tMWN</t>
+  </si>
+  <si>
+    <t>tMWN tWMAA ~tWMN</t>
+  </si>
+  <si>
+    <t>~tMWN tWMAA</t>
+  </si>
+  <si>
+    <t>MWN wMAA(-)</t>
+  </si>
+  <si>
+    <t>Positive effect of tWMAA almost exactly counterbalances negative selection into wMAA.</t>
+  </si>
+  <si>
+    <t>wMAA wMN(-)</t>
+  </si>
+  <si>
+    <t>tWMN overwhelms negative wMN</t>
+  </si>
+  <si>
+    <t>~tWMN</t>
+  </si>
+  <si>
+    <t>~MWN</t>
+  </si>
+  <si>
+    <t>~tMWN tWMN</t>
+  </si>
+  <si>
+    <t>MWN(-) wMAA</t>
+  </si>
+  <si>
+    <t>tMWN tWMN</t>
+  </si>
+  <si>
+    <t>~tMWN tWMAA tWMN</t>
+  </si>
+  <si>
+    <t>~tMWN tWMAA ~tWMN</t>
+  </si>
+  <si>
+    <t>wMAA ~wMN(-)</t>
+  </si>
+  <si>
+    <t>MWS wMAA</t>
+  </si>
+  <si>
+    <t>~tWMAA ~tWMN</t>
+  </si>
+  <si>
+    <t>~tWMAA</t>
+  </si>
+  <si>
+    <t>~wMAA</t>
+  </si>
+  <si>
+    <t>~tMWS</t>
+  </si>
+  <si>
+    <t>wMN</t>
+  </si>
+  <si>
+    <t>tWMAA tWMN(-)</t>
+  </si>
+  <si>
+    <t>tWMAA ~tWMN(-)</t>
+  </si>
+  <si>
+    <t>MWS wMAA ~wMN(-)</t>
+  </si>
+  <si>
+    <t>Positive effect of tWMN outweighs - selection into wMN.</t>
+  </si>
+  <si>
+    <t>Positive selection into wMN outweighs - selection into tWMN</t>
+  </si>
+  <si>
+    <t>~MWS wMAA</t>
+  </si>
+  <si>
+    <t>MWN wMAA wMN</t>
+  </si>
+  <si>
+    <t>~MWS wMN</t>
   </si>
 </sst>
 </file>
@@ -246,7 +336,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,8 +362,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,8 +414,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -330,6 +431,10 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -342,6 +447,10 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -671,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFB51"/>
+  <dimension ref="A1:XFB53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -969,7 +1078,7 @@
     </row>
     <row r="18" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="A18" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
@@ -977,13 +1086,13 @@
     </row>
     <row r="19" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="A19" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>20</v>
@@ -1013,7 +1122,7 @@
         <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="12" customFormat="1">
@@ -9212,7 +9321,7 @@
     </row>
     <row r="22" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="A22" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
@@ -9220,24 +9329,36 @@
         <v>35</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="B24" s="4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
@@ -9250,6 +9371,12 @@
       <c r="D25" t="s">
         <v>17</v>
       </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="B26" s="4" t="s">
@@ -9261,30 +9388,54 @@
       <c r="D26" t="s">
         <v>17</v>
       </c>
+      <c r="E26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="B29" s="4" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
@@ -9297,6 +9448,12 @@
       <c r="D30" t="s">
         <v>17</v>
       </c>
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382">
       <c r="B31" s="4" t="s">
@@ -9308,24 +9465,33 @@
       <c r="D31" t="s">
         <v>17</v>
       </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="B34" s="10" t="s">
-        <v>36</v>
+    <row r="34" spans="1:7">
+      <c r="B34" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>17</v>
@@ -9333,8 +9499,14 @@
       <c r="D34" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E34" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:7">
       <c r="B35" s="10" t="s">
         <v>19</v>
       </c>
@@ -9344,8 +9516,14 @@
       <c r="D35" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:7">
       <c r="B36" s="10" t="s">
         <v>18</v>
       </c>
@@ -9355,24 +9533,36 @@
       <c r="D36" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F36" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="B39" s="10" t="s">
-        <v>36</v>
+    <row r="39" spans="1:7">
+      <c r="B39" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C39" s="11" t="s">
         <v>17</v>
@@ -9380,8 +9570,14 @@
       <c r="D39" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:7">
       <c r="B40" s="10" t="s">
         <v>19</v>
       </c>
@@ -9391,8 +9587,14 @@
       <c r="D40" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:7">
       <c r="B41" s="10" t="s">
         <v>18</v>
       </c>
@@ -9402,24 +9604,36 @@
       <c r="D41" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:7">
       <c r="A43" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>11</v>
+        <v>40</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="B44" s="10" t="s">
-        <v>36</v>
+    <row r="44" spans="1:7">
+      <c r="B44" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>17</v>
@@ -9427,8 +9641,14 @@
       <c r="D44" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:7">
       <c r="B45" s="10" t="s">
         <v>19</v>
       </c>
@@ -9438,8 +9658,17 @@
       <c r="D45" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:7">
       <c r="B46" s="10" t="s">
         <v>18</v>
       </c>
@@ -9449,24 +9678,42 @@
       <c r="D46" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>71</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="10" t="s">
-        <v>36</v>
+    <row r="49" spans="1:6">
+      <c r="B49" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>17</v>
@@ -9474,8 +9721,14 @@
       <c r="D49" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E49" t="s">
+        <v>74</v>
+      </c>
+      <c r="F49" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="50" spans="2:4">
+    <row r="50" spans="1:6">
       <c r="B50" s="10" t="s">
         <v>19</v>
       </c>
@@ -9485,8 +9738,14 @@
       <c r="D50" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="E50" t="s">
+        <v>75</v>
+      </c>
+      <c r="F50" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="51" spans="2:4">
+    <row r="51" spans="1:6">
       <c r="B51" s="10" t="s">
         <v>18</v>
       </c>
@@ -9495,6 +9754,17 @@
       </c>
       <c r="D51" s="11" t="s">
         <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>76</v>
+      </c>
+      <c r="F51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="16" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tabulate int spec results
</commit_message>
<xml_diff>
--- a/notes/explore-results.xlsx
+++ b/notes/explore-results.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1. Exploration" sheetId="1" r:id="rId1"/>
+    <sheet name="2. Orig planned vs Int results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="96">
   <si>
     <t>Universe</t>
   </si>
@@ -251,6 +252,63 @@
   <si>
     <t>~MWS wMN</t>
   </si>
+  <si>
+    <t>DD: MWN*wMAA MWN*wMN</t>
+  </si>
+  <si>
+    <t>DD: MWS*wMAA MWS*wMN</t>
+  </si>
+  <si>
+    <t>SAME SPEC but with interactions between within-region migration and marriage</t>
+  </si>
+  <si>
+    <t>Interactions</t>
+  </si>
+  <si>
+    <t>Marr vars</t>
+  </si>
+  <si>
+    <t>tMWN</t>
+  </si>
+  <si>
+    <t>~MWN wMAA(-)</t>
+  </si>
+  <si>
+    <t>MWN wMAA ~MWN*wMAA(-)</t>
+  </si>
+  <si>
+    <t>MWN wMAA</t>
+  </si>
+  <si>
+    <t>~MWN ~wMAA(-)</t>
+  </si>
+  <si>
+    <t>tWMAA tWMN</t>
+  </si>
+  <si>
+    <t>wMAA wMN(-) MWS*wMN(-)</t>
+  </si>
+  <si>
+    <t>tMWS(-) tWMN ~tMWS*tWMN ~tMWS*tWMAA</t>
+  </si>
+  <si>
+    <t>tMWS(-) tWMAA tWMN tMWS*tWMAA</t>
+  </si>
+  <si>
+    <t>tWMAA ~tWMN</t>
+  </si>
+  <si>
+    <t>~wMAA wMN</t>
+  </si>
+  <si>
+    <t>wMN ~MWS*wMAA</t>
+  </si>
+  <si>
+    <t>~tMWS(-) tWMN</t>
+  </si>
+  <si>
+    <t>wMAA wMN</t>
+  </si>
 </sst>
 </file>
 
@@ -327,7 +385,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -335,8 +393,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -370,8 +437,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -417,8 +500,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -435,6 +526,14 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -451,6 +550,14 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -782,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -948,13 +1055,13 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" s="4" t="s">
@@ -9779,4 +9886,1025 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="41.5" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="9" max="9" width="28.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="M1" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6"/>
+      <c r="F7" s="18"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2"/>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2"/>
+      <c r="B12" s="6"/>
+      <c r="F12" s="18"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="2"/>
+      <c r="B14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="2"/>
+      <c r="B15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2"/>
+      <c r="B16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6"/>
+      <c r="F17" s="18"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="s">
+        <v>90</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="2"/>
+      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="2"/>
+      <c r="B21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="2"/>
+      <c r="B22" s="6"/>
+      <c r="F22" s="18"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="2"/>
+      <c r="B24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="2"/>
+      <c r="B25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I25" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="2"/>
+      <c r="B26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="2"/>
+      <c r="B27" s="6"/>
+      <c r="F27" s="18"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>94</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="2"/>
+      <c r="B29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="2"/>
+      <c r="B30" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>95</v>
+      </c>
+      <c r="I30" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="2"/>
+      <c r="B31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>95</v>
+      </c>
+      <c r="I31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M31" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ramsey test interacted spec
</commit_message>
<xml_diff>
--- a/notes/explore-results.xlsx
+++ b/notes/explore-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="110">
   <si>
     <t>Universe</t>
   </si>
@@ -309,12 +309,54 @@
   <si>
     <t>wMAA wMN</t>
   </si>
+  <si>
+    <t>Overall observations from the above</t>
+  </si>
+  <si>
+    <t>Gender combo not useful</t>
+  </si>
+  <si>
+    <t>Males in both regions positively select into marriage by income; in south, by status as well</t>
+  </si>
+  <si>
+    <t>Females in South positively select into marriage with Northerners by both status and income</t>
+  </si>
+  <si>
+    <t>Females in North show generally neutral selection into marriage</t>
+  </si>
+  <si>
+    <t>No systematic evidence on who migrates within regions</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Males in North gain income and status from marriage, but no particular effect from marrying northerners particularly</t>
+  </si>
+  <si>
+    <t>Males in South gain income and status from marriage, and potentially more so when marrying northerners</t>
+  </si>
+  <si>
+    <t>Male migrants within South lose income</t>
+  </si>
+  <si>
+    <t>Females in North gain income and status from marrying Northerners--perhaps less likely to drop out of labor market?</t>
+  </si>
+  <si>
+    <t>Females in South gain income and status from marrying at all, interesting, not expected</t>
+  </si>
+  <si>
+    <t>Females in South lose status by marrying Northerners</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -362,6 +404,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -454,7 +503,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -508,6 +557,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -9890,10 +9942,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10898,6 +10950,76 @@
       </c>
       <c r="M31" s="2"/>
     </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add returners to spec
</commit_message>
<xml_diff>
--- a/notes/explore-results.xlsx
+++ b/notes/explore-results.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="38400" windowHeight="24000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1. Exploration" sheetId="1" r:id="rId1"/>
     <sheet name="2. Orig planned vs Int results" sheetId="2" r:id="rId2"/>
+    <sheet name="3. Random effects results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="111">
   <si>
     <t>Universe</t>
   </si>
@@ -351,6 +352,9 @@
   <si>
     <t>Females in South lose status by marrying Northerners</t>
   </si>
+  <si>
+    <t>RANDOM EFFECTS MODEL</t>
+  </si>
 </sst>
 </file>
 
@@ -434,7 +438,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -451,8 +455,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -502,8 +515,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -560,8 +577,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -586,6 +609,8 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -610,6 +635,8 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9944,8 +9971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11029,4 +11056,228 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="6" width="55.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2"/>
+      <c r="B4" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2"/>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2"/>
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2"/>
+      <c r="B14" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2"/>
+      <c r="B15" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2"/>
+      <c r="B16" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="6"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix S spec, run, tab results
</commit_message>
<xml_diff>
--- a/notes/explore-results.xlsx
+++ b/notes/explore-results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="144">
   <si>
     <t>Universe</t>
   </si>
@@ -354,6 +354,105 @@
   </si>
   <si>
     <t>RANDOM EFFECTS MODEL</t>
+  </si>
+  <si>
+    <t>DD: MSN MR MWN</t>
+  </si>
+  <si>
+    <t>DD: WMAA WMN</t>
+  </si>
+  <si>
+    <t>Interaction terms</t>
+  </si>
+  <si>
+    <t>DD: {MSN,MR,MWN}X{WMAA,WMN}</t>
+  </si>
+  <si>
+    <t>MR(-) MWN WMAA ~MW*WMAA ~MR*WMAA ~MR*WMN(-)</t>
+  </si>
+  <si>
+    <t>tMR_tWMN(-) tMSN_tWMN</t>
+  </si>
+  <si>
+    <t>MR(-) WMAA ~MR*WMAA MR*WMN(-) ~MSN*WMN(-)</t>
+  </si>
+  <si>
+    <t>~tMWN ~tMR*tWMN ~tMSN*tWMAA tMSN*tWMN</t>
+  </si>
+  <si>
+    <t>~MR(-) MWN WMN ~MW*WMAA(-) MW*WMN ~MR*WMAA ~MSN*WMN(-)</t>
+  </si>
+  <si>
+    <t>tWMAA ~tMR*tWMN tMSN*tWMN</t>
+  </si>
+  <si>
+    <t>~MR(-) MWN ~WMAA(-) WMN ~MW*WMAA(-) MW*WMN ~MR*WMAA(-) MSN*WMAA</t>
+  </si>
+  <si>
+    <t>tMWN tWMAA ~tMSN*tWMN</t>
+  </si>
+  <si>
+    <t>~MWN WMN ~MW*WMAA(-) MR*WMN</t>
+  </si>
+  <si>
+    <t>~tMWN(-) tMWN*tWMAA</t>
+  </si>
+  <si>
+    <t>WMN</t>
+  </si>
+  <si>
+    <t>tMWN(-) ~tWMN(-) tMW*tWMAA tMR*tWMN</t>
+  </si>
+  <si>
+    <t>MR(-) MWN ~WMAA(-)  WMN ~MW*WMAA(-) MR*WMAA MR*WMN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tMWN(-) tWMAA tMW*tWMAA </t>
+  </si>
+  <si>
+    <t>~MSN MR(-) MWN MWAA(-) MWN MR*WMAA ~MR*WMN</t>
+  </si>
+  <si>
+    <t>tMWN(-) tWMAA tMW*tMAA ~tMR*tWMAA(-)</t>
+  </si>
+  <si>
+    <t>Whatever</t>
+  </si>
+  <si>
+    <t>WMAA</t>
+  </si>
+  <si>
+    <t>tMW tWMN tMW*tWMAA tMW*tWMN</t>
+  </si>
+  <si>
+    <t>WMAA ~WMN MW*WMN</t>
+  </si>
+  <si>
+    <t>tMW(-) ~tWMN tMW*tWMAA tMW*tWMN</t>
+  </si>
+  <si>
+    <t>~MW WMAA WMN</t>
+  </si>
+  <si>
+    <t>tMW*tWMN</t>
+  </si>
+  <si>
+    <t>~MW WNAA WMN</t>
+  </si>
+  <si>
+    <t>~tWMAA tMW*tWMN</t>
+  </si>
+  <si>
+    <t>~WMN</t>
+  </si>
+  <si>
+    <t>~WMAA WMN</t>
+  </si>
+  <si>
+    <t>tWMAA ~tWMN(-) ~tMW*tWMN</t>
+  </si>
+  <si>
+    <t>WMAA WMN</t>
   </si>
 </sst>
 </file>
@@ -465,8 +564,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -584,7 +685,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -611,6 +712,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -637,6 +739,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -11060,23 +11163,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="6" width="55.5" customWidth="1"/>
+    <col min="3" max="4" width="29.1640625" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="7" width="76.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="21" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
@@ -11090,183 +11195,396 @@
         <v>3</v>
       </c>
       <c r="E2" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2"/>
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2"/>
       <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2"/>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2"/>
       <c r="B14" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2"/>
       <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2"/>
       <c r="B16" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2"/>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="F18" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="F19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2"/>
       <c r="B20" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="F20" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="2"/>
       <c r="B21" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="F21" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="2"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="F23" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="2"/>
       <c r="B24" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="F24" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="2"/>
       <c r="B25" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="F25" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="2"/>
       <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="F26" t="s">
+        <v>143</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="F28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="2"/>
       <c r="B29" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:7">
       <c r="A30" s="2"/>
       <c r="B30" s="10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:7">
       <c r="A31" s="2"/>
       <c r="B31" s="10" t="s">
         <v>18</v>
@@ -11274,6 +11592,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>